<commit_message>
Finalized BOM. Next Step: Order enough parts for 5 boards, wait until all the parts and boards come in, assemble and test.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -80,6 +80,33 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/products/en?keywords=JK0654219NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE   282837-6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity   6P Terminal Block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/282837-6/A113322-ND/2187976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE   282837-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity   2P Terminal Block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/282837-2/A113320-ND/2187973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NXP PHP79NQ08LT,127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nexperia Mosfet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=PHP79NQ08LT</t>
   </si>
 </sst>
 </file>
@@ -90,11 +117,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -116,12 +144,22 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,7 +204,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,6 +222,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -204,16 +246,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
@@ -256,8 +298,8 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="n">
-        <f aca="false">C2+D2</f>
-        <v>2.37</v>
+        <f aca="false">C2*D2</f>
+        <v>0.74</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>9</v>
@@ -280,8 +322,8 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="n">
-        <f aca="false">C3+D3</f>
-        <v>3.65</v>
+        <f aca="false">C3*D3</f>
+        <v>2.65</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>9</v>
@@ -304,8 +346,8 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="n">
-        <f aca="false">C4+D4</f>
-        <v>2.53</v>
+        <f aca="false">C4*D4</f>
+        <v>1.53</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>9</v>
@@ -328,14 +370,97 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="n">
-        <f aca="false">C5+D5</f>
-        <v>13.33</v>
+        <f aca="false">C5*D5</f>
+        <v>22.66</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <f aca="false">C6*D6</f>
+        <v>9.54</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <f aca="false">C7*D7</f>
+        <v>8.32</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <f aca="false">C8*D8</f>
+        <v>6.48</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="3" t="n">
+        <f aca="false">E2+E3+E4+E5+E6+E7+E8</f>
+        <v>51.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Swapped out RJ-45 Connectors in all documents.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -76,10 +76,10 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/bourns-inc/CDSOT23-SM712/CDSOT23-SM712CT-ND/1630607</t>
   </si>
   <si>
-    <t xml:space="preserve">Pulse JK0654219NL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pulse RJ-45 Mountable connector</t>
+    <t xml:space="preserve">Amphenol ICC 54601-908WPLF  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RJ-45 Mountable connector</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/products/en?keywords=JK0654219NL</t>
@@ -267,15 +267,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.72"/>
@@ -397,7 +397,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>11.33</v>
+        <v>0.49</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>2</v>
@@ -407,7 +407,7 @@
       </c>
       <c r="F5" s="3" t="n">
         <f aca="false">C5*D5</f>
-        <v>22.66</v>
+        <v>0.98</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>10</v>
@@ -525,28 +525,48 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="5" t="s">
+      <c r="C10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="3" t="n">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="3" t="n">
         <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9</f>
-        <v>71.87</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="0" t="s">
+        <v>50.19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="0" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="0" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="0" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Found SMD resistors and radial capacitors.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -119,6 +119,42 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay Dale CRCW2010100RFKEFHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solderable size 2010 100 ohm SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/vishay-dale/CRCW2010100RFKEFHP/541-100PCT-ND/2222676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay Dale CRCW201010R0FKEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solderable size 2010 10 ohm SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/vishay-dale/CRCW201010R0FKEF/541-10.0ACCT-ND/1179050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIMA FKP0D001000B00JSSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radial 100 pF Film Cap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/wima/FKP0D001000B00JSSD/1928-1039-ND/9370034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nichicon UVK2GR47MED1TD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radial 0.1 uF Electrolytic Cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/nichicon/UVK2GR47MED1TD/493-12648-3-ND/4328849</t>
   </si>
   <si>
     <t xml:space="preserve">*Discount prices are available for the</t>
@@ -267,15 +303,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.72"/>
@@ -525,49 +561,147 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="H10" s="4"/>
+      <c r="A10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <f aca="false">C10*D10</f>
+        <v>3.48</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="4"/>
+      <c r="A11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <f aca="false">C11*D11</f>
+        <v>0.58</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="H12" s="4"/>
+      <c r="A12" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <f aca="false">C12*D12</f>
+        <v>2.1</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="H13" s="4"/>
+      <c r="A13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <f aca="false">C13*D13</f>
+        <v>0.06</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="5" t="s">
+      <c r="C14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="3" t="n">
-        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9</f>
-        <v>50.19</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="0" t="s">
-        <v>34</v>
+      <c r="F17" s="3" t="n">
+        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13</f>
+        <v>56.41</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shaved 10% off the per-board price with new terminal blocks.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -85,22 +85,19 @@
     <t xml:space="preserve">https://www.digikey.com/products/en?keywords=JK0654219NL</t>
   </si>
   <si>
-    <t xml:space="preserve">TE   282837-6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity   6P Terminal Block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/282837-6/A113322-ND/2187976</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE   282837-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity   2P Terminal Block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/282837-2/A113320-ND/2187973</t>
+    <t xml:space="preserve">DBParts 20 pc 2-pin 0.1” pitch Terminal Blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/DBParts-20pcs-Terminal-Connector-2-54mm/dp/B07NSJV6NW/ref=sxbs_sxwds-stvp?cv_ct_cx=terminal+block+assortment&amp;keywords=terminal+block+assortment&amp;pd_rd_i=B07NSJV6NW&amp;pd_rd_r=f9187fb7-4ab9-45b4-a445-3bf2b68a1d13&amp;pd_rd_w=WAjjn&amp;pd_rd_wg=olYB9&amp;pf_rd_p=a6d018ad-f20b-46c9-8920-433972c7d9b7&amp;pf_rd_r=PMA44C3EHR468DBRJFP7&amp;psc=1&amp;qid=1581446551&amp;sr=1-3-dd5817a1-1ba7-46c2-8996-f96e7b0f409c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DBParts 10 pc 6-pin 0.1” pitch Terminal Blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/DBParts-10pcs-Terminal-Connector-2-54mm/dp/B07S212CF8/ref=sr_1_26?keywords=DBParts&amp;qid=1581447002&amp;sr=8-26</t>
   </si>
   <si>
     <t xml:space="preserve">NXP PHP79NQ08LT,127</t>
@@ -261,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,6 +276,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,13 +307,12 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="40.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
@@ -358,6 +358,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D2)</f>
         <v>6</v>
       </c>
       <c r="F2" s="3" t="n">
@@ -385,6 +386,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D3)</f>
         <v>3</v>
       </c>
       <c r="F3" s="3" t="n">
@@ -412,6 +414,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D4)</f>
         <v>3</v>
       </c>
       <c r="F4" s="3" t="n">
@@ -439,6 +442,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D5)</f>
         <v>6</v>
       </c>
       <c r="F5" s="3" t="n">
@@ -457,25 +461,27 @@
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>3.18</v>
+        <v>6.99</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>3</v>
+        <f aca="false">(8)/20</f>
+        <v>0.4</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>9</v>
+        <f aca="false">_xlfn.CEILING.MATH(3*D6)</f>
+        <v>2</v>
       </c>
       <c r="F6" s="3" t="n">
         <f aca="false">C6*D6</f>
-        <v>9.54</v>
+        <v>2.796</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -484,34 +490,35 @@
         <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>8</v>
+        <v>8.99</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.3</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>24</v>
+        <f aca="false">_xlfn.CEILING.MATH(3*D7)</f>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="n">
         <f aca="false">C7*D7</f>
-        <v>8.32</v>
+        <v>2.697</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>1.08</v>
@@ -520,6 +527,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D8)</f>
         <v>18</v>
       </c>
       <c r="F8" s="3" t="n">
@@ -530,15 +538,15 @@
         <v>10</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>19.95</v>
@@ -547,6 +555,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D9)</f>
         <v>3</v>
       </c>
       <c r="F9" s="3" t="n">
@@ -557,15 +566,15 @@
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>0.58</v>
@@ -574,6 +583,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D10)</f>
         <v>18</v>
       </c>
       <c r="F10" s="3" t="n">
@@ -584,15 +594,15 @@
         <v>10</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>0.29</v>
@@ -601,6 +611,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D11)</f>
         <v>6</v>
       </c>
       <c r="F11" s="3" t="n">
@@ -611,15 +622,15 @@
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>0.7</v>
@@ -628,6 +639,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D12)</f>
         <v>9</v>
       </c>
       <c r="F12" s="3" t="n">
@@ -638,15 +650,15 @@
         <v>10</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>0.06</v>
@@ -655,6 +667,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D13)</f>
         <v>3</v>
       </c>
       <c r="F13" s="3" t="n">
@@ -665,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,29 +692,29 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="3" t="n">
         <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13</f>
-        <v>56.41</v>
+        <v>44.043</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the resistor footprints, and sourced new resistors in the BOM. Need to route the wires.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -118,22 +118,22 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537</t>
   </si>
   <si>
-    <t xml:space="preserve">Vishay Dale CRCW2010100RFKEFHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solderable size 2010 100 ohm SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/vishay-dale/CRCW2010100RFKEFHP/541-100PCT-ND/2222676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay Dale CRCW201010R0FKEF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solderable size 2010 10 ohm SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/vishay-dale/CRCW201010R0FKEF/541-10.0ACCT-ND/1179050</t>
+    <t xml:space="preserve">Stackpole Electronics RSMF2JT100R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 100 ohm 2 watt resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RSMF2JT100R/RSMF2JT100RCT-ND/2021858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stackpole Electronics  CF12JT10R0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 10 ohm ½ watt Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF12JT10R0/CF12JT10R0CT-ND/1830446</t>
   </si>
   <si>
     <t xml:space="preserve">WIMA FKP0D001000B00JSSD</t>
@@ -258,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,10 +276,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -307,7 +303,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,7 +491,7 @@
       <c r="C7" s="3" t="n">
         <v>8.99</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="E7" s="0" t="n">
@@ -577,18 +573,18 @@
         <v>33</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>0.58</v>
+        <v>0.28</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D10)</f>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="n">
         <f aca="false">C10*D10</f>
-        <v>3.48</v>
+        <v>2.52</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>10</v>
@@ -605,7 +601,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>0.29</v>
+        <v>0.1</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -616,7 +612,7 @@
       </c>
       <c r="F11" s="3" t="n">
         <f aca="false">C11*D11</f>
-        <v>0.58</v>
+        <v>0.2</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>10</v>
@@ -692,14 +688,14 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="3" t="n">
         <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13</f>
-        <v>44.043</v>
+        <v>42.703</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Changed BOM parts to better reflect the use of pin headers instead of screw terminals.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -85,19 +85,43 @@
     <t xml:space="preserve">https://www.digikey.com/products/en?keywords=JK0654219NL</t>
   </si>
   <si>
-    <t xml:space="preserve">DBParts 20 pc 2-pin 0.1” pitch Terminal Blocks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/DBParts-20pcs-Terminal-Connector-2-54mm/dp/B07NSJV6NW/ref=sxbs_sxwds-stvp?cv_ct_cx=terminal+block+assortment&amp;keywords=terminal+block+assortment&amp;pd_rd_i=B07NSJV6NW&amp;pd_rd_r=f9187fb7-4ab9-45b4-a445-3bf2b68a1d13&amp;pd_rd_w=WAjjn&amp;pd_rd_wg=olYB9&amp;pf_rd_p=a6d018ad-f20b-46c9-8920-433972c7d9b7&amp;pf_rd_r=PMA44C3EHR468DBRJFP7&amp;psc=1&amp;qid=1581446551&amp;sr=1-3-dd5817a1-1ba7-46c2-8996-f96e7b0f409c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DBParts 10 pc 6-pin 0.1” pitch Terminal Blocks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/DBParts-10pcs-Terminal-Connector-2-54mm/dp/B07S212CF8/ref=sr_1_26?keywords=DBParts&amp;qid=1581447002&amp;sr=8-26</t>
+    <t xml:space="preserve">Adam Tech MTS-02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CONN RCPT HSG 2POS 2.54MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digi-Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/adam-tech/MTS-02/2057-MTS-02-ND/9830694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity 640456-2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER VERT 2POS 2.54MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-2/A1921-ND/109003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sullin’s Connector Solutions SWH25X-NULC-S06-UU-BA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HOUSING 6POS .100 W/CRIMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/sullins-connector-solutions/SWH25X-NULC-S06-UU-BA/S9436-ND/2411481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity 640454-6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONN HEADER VERT 6POS 2.54MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640454-6/A19433-ND/258988</t>
   </si>
   <si>
     <t xml:space="preserve">NXP PHP79NQ08LT,127</t>
@@ -136,13 +160,13 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF12JT10R0/CF12JT10R0CT-ND/1830446</t>
   </si>
   <si>
-    <t xml:space="preserve">WIMA FKP0D001000B00JSSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radial 100 pF Film Cap </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/wima/FKP0D001000B00JSSD/1928-1039-ND/9370034</t>
+    <t xml:space="preserve">KEMET C315C104M5U5TA7303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radial 0.1 uF Ceramic Cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/kemet/C315C104M5U5TA7303/399-9859-1-ND/3726100</t>
   </si>
   <si>
     <t xml:space="preserve">Nichicon UVK2GR47MED1TD </t>
@@ -258,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,6 +301,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -300,15 +328,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="40.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
@@ -457,260 +486,315 @@
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>6.99</v>
+        <v>0.1</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">(8)/20</f>
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D6)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3" t="n">
         <f aca="false">C6*D6</f>
-        <v>2.796</v>
+        <v>0.4</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>8.99</v>
+        <v>0.11</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D7)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F7" s="3" t="n">
         <f aca="false">C7*D7</f>
-        <v>2.697</v>
+        <v>0.44</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>1.08</v>
+        <v>0.11</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D8)</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F8" s="3" t="n">
         <f aca="false">C8*D8</f>
-        <v>6.48</v>
+        <v>0.33</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>19.95</v>
+        <v>0.4</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D9)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F9" s="3" t="n">
         <f aca="false">C9*D9</f>
-        <v>19.95</v>
+        <v>1.2</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>0.28</v>
+        <v>1.08</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D10)</f>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3" t="n">
         <f aca="false">C10*D10</f>
-        <v>2.52</v>
+        <v>6.48</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>34</v>
+      <c r="H10" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>0.1</v>
+        <v>19.95</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D11)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F11" s="3" t="n">
         <f aca="false">C11*D11</f>
-        <v>0.2</v>
+        <v>19.95</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>0.7</v>
+        <v>0.28</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D12)</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F12" s="3" t="n">
         <f aca="false">C12*D12</f>
-        <v>2.1</v>
+        <v>2.52</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D13)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F13" s="3" t="n">
         <f aca="false">C13*D13</f>
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D14)</f>
+        <v>9</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <f aca="false">C14*D14</f>
+        <v>0.72</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="3" t="n">
         <v>0.06</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="H15" s="4"/>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D15)</f>
+        <v>3</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <f aca="false">C15*D15</f>
+        <v>0.06</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="5" t="s">
+      <c r="C16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="3" t="n">
-        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13</f>
-        <v>42.703</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="0" t="s">
-        <v>45</v>
+      <c r="F19" s="3" t="n">
+        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13+F14+F15</f>
+        <v>38.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -718,7 +802,7 @@
     <hyperlink ref="H2" r:id="rId1" display="https://www.digikey.com/product-detail/en/74HC165D%2c653/1727-2788-1-ND/763378/?itemSeq=316548520"/>
     <hyperlink ref="H3" r:id="rId2" display="https://www.digikey.com/product-detail/en/texas-instruments/SN65HVD72DR/296-39179-1-ND/5143186"/>
     <hyperlink ref="H5" r:id="rId3" display="https://www.digikey.com/products/en?keywords=JK0654219NL"/>
-    <hyperlink ref="H9" r:id="rId4" display="https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537"/>
+    <hyperlink ref="H11" r:id="rId4" display="https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Swapped out screw terminals for pin headers.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -76,15 +76,6 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/bourns-inc/CDSOT23-SM712/CDSOT23-SM712CT-ND/1630607</t>
   </si>
   <si>
-    <t xml:space="preserve">Amphenol ICC 54601-908WPLF  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RJ-45 Mountable connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=JK0654219NL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adam Tech MTS-02 </t>
   </si>
   <si>
@@ -122,6 +113,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640454-6/A19433-ND/258988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity 640454-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONN HEADER VERT 8POS 2.54MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-8/A1924-ND/109011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sullin’s Connector Solutions SWH25X-NULC-S08-UU-BA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN RCPT .100" SNGL BEIGE 8POS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/sullins-connector-solutions/SWH25X-NULC-S08-UU-BA/S9429-ND/2411483</t>
   </si>
   <si>
     <t xml:space="preserve">NXP PHP79NQ08LT,127</t>
@@ -328,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -461,49 +470,49 @@
         <v>19</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>0.49</v>
+        <v>0.1</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D5)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="n">
         <f aca="false">C5*D5</f>
-        <v>0.98</v>
+        <v>0.5</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="C6" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D6)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="n">
         <f aca="false">C6*D6</f>
-        <v>0.4</v>
+        <v>0.55</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>24</v>
@@ -531,7 +540,7 @@
         <v>0.44</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>27</v>
@@ -541,25 +550,25 @@
       <c r="A8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="0" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>0.11</v>
+        <v>0.4</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D8)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="n">
         <f aca="false">C8*D8</f>
-        <v>0.33</v>
+        <v>1.6</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>30</v>
@@ -573,55 +582,55 @@
         <v>32</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D9)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F9" s="3" t="n">
         <f aca="false">C9*D9</f>
-        <v>1.2</v>
+        <v>0.44</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>1.08</v>
+        <v>0.15</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D10)</f>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F10" s="3" t="n">
         <f aca="false">C10*D10</f>
-        <v>6.48</v>
+        <v>0.15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>37</v>
       </c>
@@ -629,23 +638,23 @@
         <v>38</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>19.95</v>
+        <v>1.08</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D11)</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F11" s="3" t="n">
         <f aca="false">C11*D11</f>
-        <v>19.95</v>
+        <v>6.48</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="0" t="s">
         <v>39</v>
       </c>
     </row>
@@ -657,18 +666,18 @@
         <v>41</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>0.28</v>
+        <v>19.95</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D12)</f>
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="F12" s="3" t="n">
         <f aca="false">C12*D12</f>
-        <v>2.52</v>
+        <v>19.95</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>10</v>
@@ -685,18 +694,18 @@
         <v>44</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>0.1</v>
+        <v>0.28</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D13)</f>
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F13" s="3" t="n">
         <f aca="false">C13*D13</f>
-        <v>0.2</v>
+        <v>2.52</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>10</v>
@@ -713,18 +722,18 @@
         <v>47</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D14)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F14" s="3" t="n">
         <f aca="false">C14*D14</f>
-        <v>0.72</v>
+        <v>0.2</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>10</v>
@@ -741,18 +750,18 @@
         <v>50</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>0.06</v>
+        <v>0.24</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D15)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F15" s="3" t="n">
         <f aca="false">C15*D15</f>
-        <v>0.06</v>
+        <v>0.72</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>10</v>
@@ -762,9 +771,32 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="H16" s="4"/>
+      <c r="A16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D16)</f>
+        <v>3</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <f aca="false">C16*D16</f>
+        <v>0.06</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="3"/>
@@ -772,37 +804,41 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="6" t="s">
+      <c r="C18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="3" t="n">
-        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13+F14+F15</f>
-        <v>38.2</v>
-      </c>
-    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="0" t="s">
-        <v>52</v>
+      <c r="F20" s="3" t="n">
+        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13+F14+F15+F16</f>
+        <v>38.53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F22" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="https://www.digikey.com/product-detail/en/74HC165D%2c653/1727-2788-1-ND/763378/?itemSeq=316548520"/>
     <hyperlink ref="H3" r:id="rId2" display="https://www.digikey.com/product-detail/en/texas-instruments/SN65HVD72DR/296-39179-1-ND/5143186"/>
-    <hyperlink ref="H5" r:id="rId3" display="https://www.digikey.com/products/en?keywords=JK0654219NL"/>
-    <hyperlink ref="H11" r:id="rId4" display="https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537"/>
+    <hyperlink ref="H12" r:id="rId3" display="https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added parts to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -151,15 +151,6 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537</t>
   </si>
   <si>
-    <t xml:space="preserve">Stackpole Electronics RSMF2JT100R </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Through Hole 100 ohm 2 watt resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RSMF2JT100R/RSMF2JT100RCT-ND/2021858</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stackpole Electronics  CF12JT10R0 </t>
   </si>
   <si>
@@ -167,6 +158,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF12JT10R0/CF12JT10R0CT-ND/1830446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stackpole Electronics  CF14JT100R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 100 ohm ¼ watt Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT100R/CF14JT100RCT-ND/1830327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stackpole Electronics  CF18JT3K00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 3k ohm 1/4 watt Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF18JT3K00/CF18JT3K00CT-ND/2022753</t>
   </si>
   <si>
     <t xml:space="preserve">KEMET C315C104M5U5TA7303</t>
@@ -337,10 +346,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -694,18 +703,18 @@
         <v>44</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>0.28</v>
+        <v>0.1</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D13)</f>
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="F13" s="3" t="n">
         <f aca="false">C13*D13</f>
-        <v>2.52</v>
+        <v>0.2</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>10</v>
@@ -725,15 +734,15 @@
         <v>0.1</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D14)</f>
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="F14" s="3" t="n">
         <f aca="false">C14*D14</f>
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>10</v>
@@ -750,18 +759,18 @@
         <v>50</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D15)</f>
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="F15" s="3" t="n">
         <f aca="false">C15*D15</f>
-        <v>0.72</v>
+        <v>1.4</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>10</v>
@@ -778,18 +787,18 @@
         <v>53</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>0.06</v>
+        <v>0.24</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D16)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F16" s="3" t="n">
         <f aca="false">C16*D16</f>
-        <v>0.06</v>
+        <v>0.72</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>10</v>
@@ -799,9 +808,32 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="H17" s="4"/>
+      <c r="A17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D17)</f>
+        <v>3</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <f aca="false">C17*D17</f>
+        <v>0.06</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="3"/>
@@ -809,29 +841,34 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="6" t="s">
+      <c r="C19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="3" t="n">
-        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13+F14+F15+F16</f>
-        <v>38.53</v>
-      </c>
-    </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="0" t="s">
-        <v>55</v>
+      <c r="F21" s="3" t="n">
+        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13+F14+F15+F16+F17</f>
+        <v>38.81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F22" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F23" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>